<commit_message>
new mode choice estimation
</commit_message>
<xml_diff>
--- a/input/estimation_results_mode.xlsx
+++ b/input/estimation_results_mode.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.arnz\Code\quetzal_germany\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.arnz\Code\quetzal_germany\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2C3D42-E9F3-4FD7-AE8E-15D1013DBA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E7974E-3849-41FF-9568-E253414C2581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38490" yWindow="-10700" windowWidth="19380" windowHeight="20970" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leisure_no_car" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="commuting_no_car" sheetId="3" r:id="rId3"/>
     <sheet name="commuting_car" sheetId="4" r:id="rId4"/>
     <sheet name="buy-execute_no_car" sheetId="5" r:id="rId5"/>
-    <sheet name="buy-execute_car" sheetId="6" r:id="rId6"/>
+    <sheet name="buy-execute_car" sheetId="13" r:id="rId6"/>
     <sheet name="business_no_car" sheetId="7" r:id="rId7"/>
     <sheet name="business_car" sheetId="8" r:id="rId8"/>
     <sheet name="accompany_no_car" sheetId="9" r:id="rId9"/>
@@ -476,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -499,16 +499,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-5.1707539713218464</v>
+        <v>-5.0532471948770334</v>
       </c>
       <c r="C2">
-        <v>0.83883857401377182</v>
+        <v>0.8423170926111595</v>
       </c>
       <c r="D2">
-        <v>-6.1641823963581261</v>
+        <v>-5.9992219547772763</v>
       </c>
       <c r="E2">
-        <v>7.0848238387100082E-10</v>
+        <v>1.9826520425425538E-9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -516,13 +516,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2.4810830089139659</v>
+        <v>2.3946479373023748</v>
       </c>
       <c r="C3">
-        <v>0.25863213869395119</v>
+        <v>0.25364665151762811</v>
       </c>
       <c r="D3">
-        <v>9.5930962851060109</v>
+        <v>9.4408813322574101</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -533,16 +533,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.24255747606623901</v>
+        <v>0.1746574554607187</v>
       </c>
       <c r="C4">
-        <v>0.38978266841651832</v>
+        <v>0.39235288652958328</v>
       </c>
       <c r="D4">
-        <v>0.62228902339763403</v>
+        <v>0.44515399645861808</v>
       </c>
       <c r="E4">
-        <v>0.5337518375471888</v>
+        <v>0.65620846945821842</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -550,16 +550,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-1.247569742054808</v>
+        <v>-1.2861372537428011</v>
       </c>
       <c r="C5">
-        <v>0.4228786495845972</v>
+        <v>0.42401948097833952</v>
       </c>
       <c r="D5">
-        <v>-2.9501838016185551</v>
+        <v>-3.0332032169260201</v>
       </c>
       <c r="E5">
-        <v>3.1758493557125789E-3</v>
+        <v>2.4197259197851211E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -567,16 +567,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.5370900516963659</v>
+        <v>1.609563568270123</v>
       </c>
       <c r="C6">
-        <v>0.21664018031413779</v>
+        <v>0.21656942750414851</v>
       </c>
       <c r="D6">
-        <v>7.0951291190190018</v>
+        <v>7.4320904239324879</v>
       </c>
       <c r="E6">
-        <v>1.292299600663682E-12</v>
+        <v>1.068034549689401E-13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -584,13 +584,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2.1575931767252619</v>
+        <v>2.1605154875823098</v>
       </c>
       <c r="C7">
-        <v>0.20642208576122181</v>
+        <v>0.20660568867638321</v>
       </c>
       <c r="D7">
-        <v>10.45233686486945</v>
+        <v>10.457192642775841</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -601,16 +601,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-6.1651702763098941E-2</v>
+        <v>-6.3723847274516507E-2</v>
       </c>
       <c r="C8">
-        <v>1.588991186330297E-2</v>
+        <v>1.5931690302559001E-2</v>
       </c>
       <c r="D8">
-        <v>-3.8799272955994648</v>
+        <v>-3.9998170981443799</v>
       </c>
       <c r="E8">
-        <v>1.04487692546229E-4</v>
+        <v>6.3391457171713128E-5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -618,16 +618,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-1.6282500782410621E-2</v>
+        <v>-1.3692568852585451E-2</v>
       </c>
       <c r="C9">
-        <v>4.53010689640671E-3</v>
+        <v>4.491265495140266E-3</v>
       </c>
       <c r="D9">
-        <v>-3.594286217688579</v>
+        <v>-3.0487106289755901</v>
       </c>
       <c r="E9">
-        <v>3.2528210319626721E-4</v>
+        <v>2.2982573959966501E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -643,7 +643,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -659,7 +659,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-506.88329181639727</v>
+        <v>-508.08731953450052</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -670,7 +670,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-348.69803904571631</v>
+        <v>-351.7223271678256</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -681,7 +681,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>316.37050554136192</v>
+        <v>312.72998473334968</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -692,7 +692,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.31207430847410661</v>
+        <v>0.30775220391237751</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -703,7 +703,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.29629158268858652</v>
+        <v>0.29200687886208998</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -714,7 +714,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>713.39607809143263</v>
+        <v>719.44465433565119</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -725,7 +725,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>744.95944296028529</v>
+        <v>751.07060100995352</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -736,7 +736,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.5774010602556811E-3</v>
+        <v>1.111233066012662E-3</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -759,7 +759,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -799,16 +801,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-2.9728901978752398</v>
+        <v>-2.46396062168012</v>
       </c>
       <c r="C3">
-        <v>0.27230002319391611</v>
+        <v>0.31507374511365782</v>
       </c>
       <c r="D3">
-        <v>-10.91770086173706</v>
+        <v>-7.820266397605697</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>5.3290705182007514E-15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -816,16 +818,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-5.1106911780923641</v>
+        <v>-4.7096472146805333</v>
       </c>
       <c r="C4">
-        <v>1.293747785489656</v>
+        <v>1.3027537243626639</v>
       </c>
       <c r="D4">
-        <v>-3.9502994597653172</v>
+        <v>-3.6151477647738819</v>
       </c>
       <c r="E4">
-        <v>7.8053473551387142E-5</v>
+        <v>3.0017635771706352E-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -833,13 +835,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-5.696594697855736</v>
+        <v>-5.2843699536352764</v>
       </c>
       <c r="C5">
-        <v>0.31799980830479951</v>
+        <v>0.35106059290572689</v>
       </c>
       <c r="D5">
-        <v>-17.9138306033053</v>
+        <v>-15.05258653469639</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -850,16 +852,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-4.4864721476554994</v>
+        <v>-4.4617519202945592</v>
       </c>
       <c r="C6">
-        <v>2.116033250587952</v>
+        <v>2.1435383185895018</v>
       </c>
       <c r="D6">
-        <v>-2.1202276223253622</v>
+        <v>-2.0814892281610788</v>
       </c>
       <c r="E6">
-        <v>3.3986854031629272E-2</v>
+        <v>3.7389149047711179E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -867,13 +869,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-4.0267932892770268</v>
+        <v>-3.818045990882974</v>
       </c>
       <c r="C7">
-        <v>0.20286259077332919</v>
+        <v>0.22365305165472429</v>
       </c>
       <c r="D7">
-        <v>-19.84985636793138</v>
+        <v>-17.07128949341266</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -884,16 +886,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-0.22316119704791509</v>
+        <v>-0.21722483227643821</v>
       </c>
       <c r="C8">
-        <v>3.9167257833603218E-2</v>
+        <v>3.9559756839046979E-2</v>
       </c>
       <c r="D8">
-        <v>-5.6976466924487088</v>
+        <v>-5.4910558009807851</v>
       </c>
       <c r="E8">
-        <v>1.214724520970378E-8</v>
+        <v>3.9953808705917033E-8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -901,16 +903,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-2.8594717581299962E-2</v>
+        <v>-4.1132003975000157E-2</v>
       </c>
       <c r="C9">
-        <v>6.6057475919595026E-3</v>
+        <v>8.5269513949378737E-3</v>
       </c>
       <c r="D9">
-        <v>-4.3287632751977041</v>
+        <v>-4.8237643291151713</v>
       </c>
       <c r="E9">
-        <v>1.499490037559781E-5</v>
+        <v>1.40873859333368E-6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -926,7 +928,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>5093</v>
+        <v>5246</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -942,7 +944,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-6225.6405330717162</v>
+        <v>-6437.880550479701</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -953,7 +955,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-447.46532797846959</v>
+        <v>-439.06028147952469</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -964,7 +966,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>11556.350410186489</v>
+        <v>11997.640538000351</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -975,7 +977,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.92812541527229953</v>
+        <v>0.93180049271855325</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -986,7 +988,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.92684040693339809</v>
+        <v>0.93055784773045946</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -997,7 +999,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>910.93065595693918</v>
+        <v>894.12056295904949</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1008,7 +1010,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>963.21563457201603</v>
+        <v>946.64233224246402</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1019,7 +1021,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.9821716780742051E-4</v>
+        <v>1.133524761551212E-4</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1042,7 +1044,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1082,16 +1086,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.813865365397872</v>
+        <v>1.86045471497878</v>
       </c>
       <c r="C3">
-        <v>0.57048077697556188</v>
+        <v>0.55770510369216619</v>
       </c>
       <c r="D3">
-        <v>3.1795380994504119</v>
+        <v>3.3359112238027619</v>
       </c>
       <c r="E3">
-        <v>1.475099765126497E-3</v>
+        <v>8.5020308899474983E-4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1099,16 +1103,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1.000692030006304</v>
+        <v>0.95081138431308654</v>
       </c>
       <c r="C4">
-        <v>0.86886640378415936</v>
+        <v>0.85166473594446135</v>
       </c>
       <c r="D4">
-        <v>1.1517213988802031</v>
+        <v>1.1164151152256829</v>
       </c>
       <c r="E4">
-        <v>0.24943557600459521</v>
+        <v>0.26424448641742432</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1116,16 +1120,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-4.0021229169575907</v>
+        <v>-4.1145883589905523</v>
       </c>
       <c r="C5">
-        <v>1.83686878885498</v>
+        <v>1.8437366401560471</v>
       </c>
       <c r="D5">
-        <v>-2.178774521751405</v>
+        <v>-2.2316573144862542</v>
       </c>
       <c r="E5">
-        <v>2.934842255890446E-2</v>
+        <v>2.5637620462940051E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1133,16 +1137,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-3.594335977228929E-3</v>
+        <v>6.8728850869433034E-2</v>
       </c>
       <c r="C6">
-        <v>1.370579430979201</v>
+        <v>1.3700185015651249</v>
       </c>
       <c r="D6">
-        <v>-2.6224937394989079E-3</v>
+        <v>5.0166366943888999E-2</v>
       </c>
       <c r="E6">
-        <v>0.99790755513290752</v>
+        <v>0.95998981308267251</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1150,16 +1154,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.1911598575306499</v>
+        <v>1.234593408829292</v>
       </c>
       <c r="C7">
-        <v>0.46678800566357281</v>
+        <v>0.47177831564464912</v>
       </c>
       <c r="D7">
-        <v>2.5518219043296329</v>
+        <v>2.6168930785687219</v>
       </c>
       <c r="E7">
-        <v>1.07161280400152E-2</v>
+        <v>8.8734131505059377E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1167,16 +1171,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-8.2924104646101157E-2</v>
+        <v>-8.385236116477586E-2</v>
       </c>
       <c r="C8">
-        <v>5.6232939362574112E-2</v>
+        <v>5.6163160810944801E-2</v>
       </c>
       <c r="D8">
-        <v>-1.4746535675723791</v>
+        <v>-1.4930135689306701</v>
       </c>
       <c r="E8">
-        <v>0.1403057053762797</v>
+        <v>0.13543363509348261</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1184,16 +1188,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-4.1784521231371101E-2</v>
+        <v>-3.4084377185844963E-2</v>
       </c>
       <c r="C9">
-        <v>3.0787220027029071E-2</v>
+        <v>3.018770220858499E-2</v>
       </c>
       <c r="D9">
-        <v>-1.3572034498303891</v>
+        <v>-1.129081536260544</v>
       </c>
       <c r="E9">
-        <v>0.17471657490300399</v>
+        <v>0.25886343940846679</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1209,7 +1213,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1225,7 +1229,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-159.31819437073531</v>
+        <v>-168.70704678905281</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1236,7 +1240,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-100.3866206003476</v>
+        <v>-104.2569847307753</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1247,7 +1251,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>117.8631475407752</v>
+        <v>128.90012411655511</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1258,7 +1262,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.36989857940049942</v>
+        <v>0.38202353301142389</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1269,7 +1273,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.31968460332828819</v>
+        <v>0.33460405556657841</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -1280,7 +1284,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>216.77324120069531</v>
+        <v>224.51396946155049</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1291,7 +1295,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>234.410782155823</v>
+        <v>242.3868214983286</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1302,7 +1306,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>2.2922862643168091E-4</v>
+        <v>7.4054413197065249E-4</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1325,7 +1329,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1365,13 +1371,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.82541626204953222</v>
+        <v>0.87468872115164675</v>
       </c>
       <c r="C3">
-        <v>8.3967491889938364E-2</v>
+        <v>9.5767107594211184E-2</v>
       </c>
       <c r="D3">
-        <v>9.8301883677966568</v>
+        <v>9.1334983704208579</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1382,16 +1388,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-0.8532961815452742</v>
+        <v>-0.81426292023067048</v>
       </c>
       <c r="C4">
-        <v>0.2299322486720741</v>
+        <v>0.22143532529444729</v>
       </c>
       <c r="D4">
-        <v>-3.7110765735268059</v>
+        <v>-3.6772042543254</v>
       </c>
       <c r="E4">
-        <v>2.0637965727710039E-4</v>
+        <v>2.3580422134528159E-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1399,13 +1405,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-3.0506026401556561</v>
+        <v>-2.727770620754479</v>
       </c>
       <c r="C5">
-        <v>0.188849004575639</v>
+        <v>0.18043216670388659</v>
       </c>
       <c r="D5">
-        <v>-16.153660153044701</v>
+        <v>-15.117984063402149</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1416,16 +1422,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-2.433511605392026</v>
+        <v>-2.628210351262092</v>
       </c>
       <c r="C6">
-        <v>0.51729675161243804</v>
+        <v>0.51809890491310606</v>
       </c>
       <c r="D6">
-        <v>-4.7042854953305948</v>
+        <v>-5.0727965767518608</v>
       </c>
       <c r="E6">
-        <v>2.547565516097805E-6</v>
+        <v>3.9201149504286548E-7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1433,16 +1439,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-0.36664539771371529</v>
+        <v>-0.29332225431651282</v>
       </c>
       <c r="C7">
-        <v>6.5207696423486436E-2</v>
+        <v>7.0749046755809258E-2</v>
       </c>
       <c r="D7">
-        <v>-5.6227319445938493</v>
+        <v>-4.1459534476685773</v>
       </c>
       <c r="E7">
-        <v>1.8796094458650711E-8</v>
+        <v>3.3840258093720272E-5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1450,16 +1456,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-5.0634376303862652E-2</v>
+        <v>-3.3921924421893443E-2</v>
       </c>
       <c r="C8">
-        <v>9.2188822196681754E-3</v>
+        <v>8.8236872345383993E-3</v>
       </c>
       <c r="D8">
-        <v>-5.4924637388072828</v>
+        <v>-3.8444160043562592</v>
       </c>
       <c r="E8">
-        <v>3.9636495197115102E-8</v>
+        <v>1.20839865210165E-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1467,13 +1473,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-4.2094905370716848E-2</v>
+        <v>-3.972621361058884E-2</v>
       </c>
       <c r="C9">
-        <v>4.4320877248411493E-3</v>
+        <v>4.4745437749785909E-3</v>
       </c>
       <c r="D9">
-        <v>-9.4977599686896053</v>
+        <v>-8.8782713072862744</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1492,7 +1498,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>2519</v>
+        <v>2589</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1508,7 +1514,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-3258.6946965225652</v>
+        <v>-3334.025990199621</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1519,7 +1525,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-2550.2749651990298</v>
+        <v>-2636.2555675374701</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1530,7 +1536,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>1416.8394626470699</v>
+        <v>1395.5408453243019</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1541,7 +1547,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.21739371045698369</v>
+        <v>0.20928763744291409</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1552,7 +1558,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.21493873975704761</v>
+        <v>0.20688813605224829</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -1563,7 +1569,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>5116.5499303980596</v>
+        <v>5288.5111350749394</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1574,7 +1580,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>5163.2028686088825</v>
+        <v>5335.3833509129518</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1585,7 +1591,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>2.6228064331088551E-4</v>
+        <v>4.6615943184417328E-4</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1631,16 +1637,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.49578434846551439</v>
+        <v>0.12443955808591391</v>
       </c>
       <c r="C2">
-        <v>0.56666298132364479</v>
+        <v>0.59969315623044994</v>
       </c>
       <c r="D2">
-        <v>0.87491924619362305</v>
+        <v>0.20750538303307611</v>
       </c>
       <c r="E2">
-        <v>0.38161784621069011</v>
+        <v>0.83561518911108346</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1648,13 +1654,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-2.7115366664987581</v>
+        <v>-2.470159158229102</v>
       </c>
       <c r="C3">
-        <v>6.9407433461250015E-2</v>
+        <v>8.1628130977825147E-2</v>
       </c>
       <c r="D3">
-        <v>-39.066949046784757</v>
+        <v>-30.261126019167801</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1665,13 +1671,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-3.2955705568455129</v>
+        <v>-2.8858598474839061</v>
       </c>
       <c r="C4">
-        <v>0.20803975971888419</v>
+        <v>0.18851576250138141</v>
       </c>
       <c r="D4">
-        <v>-15.841061157245541</v>
+        <v>-15.30832122042187</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1682,13 +1688,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-3.7339516664324548</v>
+        <v>-3.5838579737122669</v>
       </c>
       <c r="C5">
-        <v>7.7273226682782983E-2</v>
+        <v>8.2243930221597594E-2</v>
       </c>
       <c r="D5">
-        <v>-48.321415148882423</v>
+        <v>-43.57595708347035</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1699,13 +1705,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-2.938052922846643</v>
+        <v>-2.5965508934771209</v>
       </c>
       <c r="C6">
-        <v>0.1852083546335406</v>
+        <v>0.22726057369729799</v>
       </c>
       <c r="D6">
-        <v>-15.86350102110659</v>
+        <v>-11.42543491479355</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1716,13 +1722,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-2.6271068494125491</v>
+        <v>-2.4594236893706301</v>
       </c>
       <c r="C7">
-        <v>5.1264698585735603E-2</v>
+        <v>5.9630816451050207E-2</v>
       </c>
       <c r="D7">
-        <v>-51.245924035210088</v>
+        <v>-41.244172656759183</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1733,16 +1739,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-1.5400475769532219E-2</v>
+        <v>-2.6894443092045878E-2</v>
       </c>
       <c r="C8">
-        <v>7.5002880837191123E-3</v>
+        <v>1.15425278910396E-2</v>
       </c>
       <c r="D8">
-        <v>-2.053317898943384</v>
+        <v>-2.330030591732327</v>
       </c>
       <c r="E8">
-        <v>4.0041756041985899E-2</v>
+        <v>1.9804534312010121E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1750,13 +1756,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-1.356189078493575E-2</v>
+        <v>-1.8364013070772858E-2</v>
       </c>
       <c r="C9">
-        <v>1.4601148302692359E-3</v>
+        <v>1.5508245659285849E-3</v>
       </c>
       <c r="D9">
-        <v>-9.2882357632344714</v>
+        <v>-11.84145097661454</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1775,7 +1781,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>16534</v>
+        <v>17197</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1791,7 +1797,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-18504.517696257361</v>
+        <v>-19159.529429758459</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1802,7 +1808,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-5543.2835362950464</v>
+        <v>-5564.1730354486908</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1813,7 +1819,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>25922.468319924628</v>
+        <v>27190.712788619541</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1824,7 +1830,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.70043620551017094</v>
+        <v>0.70958717666591264</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1835,7 +1841,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.70000387865186975</v>
+        <v>0.70916962987650267</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -1846,7 +1852,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>11102.567072590091</v>
+        <v>11144.34607089738</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1857,7 +1863,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>11164.27246575659</v>
+        <v>11206.365992729259</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1868,7 +1874,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>2.391603705420765E-2</v>
+        <v>1.9957920849218599E-2</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1891,7 +1897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1931,16 +1939,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.3876522909573139</v>
+        <v>1.3424267654694899</v>
       </c>
       <c r="C3">
-        <v>0.2060729686016263</v>
+        <v>0.20680535299576791</v>
       </c>
       <c r="D3">
-        <v>6.7337909497478972</v>
+        <v>6.4912573394411188</v>
       </c>
       <c r="E3">
-        <v>1.6529888569039031E-11</v>
+        <v>8.5123019744060002E-11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1948,16 +1956,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-0.79090312113736905</v>
+        <v>-0.9845398117062335</v>
       </c>
       <c r="C4">
-        <v>0.32407654754152648</v>
+        <v>0.3392098615863407</v>
       </c>
       <c r="D4">
-        <v>-2.4404824327376682</v>
+        <v>-2.902450439093835</v>
       </c>
       <c r="E4">
-        <v>1.466765932255365E-2</v>
+        <v>3.702557402778472E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1965,16 +1973,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-2.945991955908851</v>
+        <v>-2.8942148064322888</v>
       </c>
       <c r="C5">
-        <v>0.56033431031174952</v>
+        <v>0.55861222683102474</v>
       </c>
       <c r="D5">
-        <v>-5.2575612481588161</v>
+        <v>-5.1810803047598943</v>
       </c>
       <c r="E5">
-        <v>1.4597828412732381E-7</v>
+        <v>2.206044844577093E-7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1982,16 +1990,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.62298425056701612</v>
+        <v>0.74071104863284765</v>
       </c>
       <c r="C6">
-        <v>0.48459421760540788</v>
+        <v>0.47040726699080188</v>
       </c>
       <c r="D6">
-        <v>1.2855792081990871</v>
+        <v>1.574616509160627</v>
       </c>
       <c r="E6">
-        <v>0.19858995687448019</v>
+        <v>0.1153449898155807</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1999,13 +2007,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.7262585355218969</v>
+        <v>1.7956168040361971</v>
       </c>
       <c r="C7">
-        <v>0.1971374972351001</v>
+        <v>0.19571380491900761</v>
       </c>
       <c r="D7">
-        <v>8.7566219503294906</v>
+        <v>9.1747069389370779</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2016,16 +2024,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-4.2378251828333602E-2</v>
+        <v>-4.101186323576636E-2</v>
       </c>
       <c r="C8">
-        <v>2.9259155125177821E-2</v>
+        <v>2.7278725849460759E-2</v>
       </c>
       <c r="D8">
-        <v>-1.4483757868957281</v>
+        <v>-1.503437640822842</v>
       </c>
       <c r="E8">
-        <v>0.1475119826947098</v>
+        <v>0.13272622623234051</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2033,16 +2041,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>1.000541552297111E-3</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>2.4107208790535069E-3</v>
+        <v>2.5004850056551879E-3</v>
       </c>
       <c r="D9">
-        <v>0.41503832359470061</v>
+        <v>1.2685481246163619</v>
       </c>
       <c r="E9">
-        <v>0.67811384848607714</v>
+        <v>0.2046022762196282</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -2058,7 +2066,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>364</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2074,7 +2082,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-628.586824854253</v>
+        <v>-609.83515302317971</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -2085,7 +2093,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-416.93932099809172</v>
+        <v>-404.49857100579987</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -2096,7 +2104,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>423.29500771232262</v>
+        <v>410.67316403475962</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -2107,7 +2115,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.3367036907037223</v>
+        <v>0.33670833994965688</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -2118,7 +2126,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.32397672971173058</v>
+        <v>0.32359004074971559</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2129,7 +2137,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>849.87864199618343</v>
+        <v>824.99714201159986</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -2140,7 +2148,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>881.0558729372774</v>
+        <v>855.88343179932679</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -2151,7 +2159,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.28147358666789E-6</v>
+        <v>9.3213283476952999E-7</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -2174,7 +2182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2214,13 +2224,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-1.8550747910787959</v>
+        <v>-1.818434104221158</v>
       </c>
       <c r="C3">
-        <v>8.026411612927449E-2</v>
+        <v>8.4450303317423897E-2</v>
       </c>
       <c r="D3">
-        <v>-23.112131305239661</v>
+        <v>-21.532594114981421</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2231,13 +2241,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-5.4275308240651912</v>
+        <v>-5.2444468548668262</v>
       </c>
       <c r="C4">
-        <v>0.46626016808499249</v>
+        <v>0.43483331359388933</v>
       </c>
       <c r="D4">
-        <v>-11.640562920819409</v>
+        <v>-12.060821217954921</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2248,13 +2258,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-6.3628072470941071</v>
+        <v>-6.2916545775286998</v>
       </c>
       <c r="C5">
-        <v>0.24123621343380369</v>
+        <v>0.2458395768574953</v>
       </c>
       <c r="D5">
-        <v>-26.37583784177615</v>
+        <v>-25.592521179678709</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2265,16 +2275,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.31921659188296703</v>
+        <v>0.30254715379359809</v>
       </c>
       <c r="C6">
-        <v>0.1827755582981514</v>
+        <v>0.18117736288328801</v>
       </c>
       <c r="D6">
-        <v>1.7464949627578059</v>
+        <v>1.669894897347054</v>
       </c>
       <c r="E6">
-        <v>8.0724981610890811E-2</v>
+        <v>9.4940160089753922E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2282,13 +2292,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-1.9729785855957951</v>
+        <v>-1.905261796000334</v>
       </c>
       <c r="C7">
-        <v>3.8152883051168193E-2</v>
+        <v>4.0901425394536867E-2</v>
       </c>
       <c r="D7">
-        <v>-51.712437640682687</v>
+        <v>-46.581794585936763</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2299,13 +2309,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-0.23421468141964011</v>
+        <v>-0.22834182345483409</v>
       </c>
       <c r="C8">
-        <v>9.1461014376677443E-3</v>
+        <v>9.1512028005063459E-3</v>
       </c>
       <c r="D8">
-        <v>-25.60814386499576</v>
+        <v>-24.95211049657863</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2316,13 +2326,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-1.332767935891473E-2</v>
+        <v>-1.380099840461871E-2</v>
       </c>
       <c r="C9">
-        <v>1.237387527066341E-3</v>
+        <v>1.2488932629084639E-3</v>
       </c>
       <c r="D9">
-        <v>-10.77082083614715</v>
+        <v>-11.05058279558534</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2341,7 +2351,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>14584</v>
+        <v>14898</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2357,7 +2367,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-17106.531654401741</v>
+        <v>-17465.86759717411</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -2368,7 +2378,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-4935.6338622507919</v>
+        <v>-4914.450725121379</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -2379,7 +2389,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>24341.79558430189</v>
+        <v>25102.833744105461</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -2390,7 +2400,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.71147664751897333</v>
+        <v>0.71862544486959745</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -2401,7 +2411,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.71100898989195571</v>
+        <v>0.71816740864806472</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2412,7 +2422,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>9887.2677245015839</v>
+        <v>9844.9014502427581</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -2423,7 +2433,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>9947.9691670324519</v>
+        <v>9905.7733082806481</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -2434,7 +2444,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.32152692429794E-2</v>
+        <v>1.018034693309005E-2</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -2457,7 +2467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2497,16 +2509,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2.154857180169595</v>
+        <v>2.046759948579826</v>
       </c>
       <c r="C3">
-        <v>0.29732071206603822</v>
+        <v>0.26758952740363617</v>
       </c>
       <c r="D3">
-        <v>7.2475851587863058</v>
+        <v>7.648879118847062</v>
       </c>
       <c r="E3">
-        <v>4.2432724001173478E-13</v>
+        <v>2.0206059048177849E-14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2514,16 +2526,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1.181975757500354</v>
+        <v>1.426902315030546</v>
       </c>
       <c r="C4">
-        <v>0.46254577041836697</v>
+        <v>0.44024364321102238</v>
       </c>
       <c r="D4">
-        <v>2.5553703721715388</v>
+        <v>3.2411650617442018</v>
       </c>
       <c r="E4">
-        <v>1.060748625212349E-2</v>
+        <v>1.190422332844054E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -2531,16 +2543,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-1.193748384951494</v>
+        <v>-1.38646927575381</v>
       </c>
       <c r="C5">
-        <v>0.42465439766041663</v>
+        <v>0.3799564701572134</v>
       </c>
       <c r="D5">
-        <v>-2.8111056697594812</v>
+        <v>-3.6490213607367559</v>
       </c>
       <c r="E5">
-        <v>4.937156820284061E-3</v>
+        <v>2.632412173892984E-4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2548,16 +2560,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-3.4833841075101319</v>
+        <v>-3.3199784516519322</v>
       </c>
       <c r="C6">
-        <v>1.008310960750429</v>
+        <v>0.89476720981145863</v>
       </c>
       <c r="D6">
-        <v>-3.4546724602870991</v>
+        <v>-3.7104382181724151</v>
       </c>
       <c r="E6">
-        <v>5.5096171709778652E-4</v>
+        <v>2.0690078701512959E-4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2565,16 +2577,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.3402995547916701</v>
+        <v>1.2327854637953739</v>
       </c>
       <c r="C7">
-        <v>0.30770450385678588</v>
+        <v>0.25037184609388841</v>
       </c>
       <c r="D7">
-        <v>4.3558008998642466</v>
+        <v>4.9238182448560313</v>
       </c>
       <c r="E7">
-        <v>1.325812483599087E-5</v>
+        <v>8.487167080239999E-7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2582,16 +2594,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>2.7358015829767521E-2</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>4.1054337773614342E-2</v>
+        <v>3.1191018598676509E-2</v>
       </c>
       <c r="D8">
-        <v>0.66638551036013904</v>
+        <v>0.29386688574690378</v>
       </c>
       <c r="E8">
-        <v>0.50516472156992021</v>
+        <v>0.76885962276917574</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2599,16 +2611,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-7.5696085601165364E-2</v>
+        <v>-8.3397779283480508E-2</v>
       </c>
       <c r="C9">
-        <v>1.327068090153821E-2</v>
+        <v>1.234875451541808E-2</v>
       </c>
       <c r="D9">
-        <v>-5.7040091735150842</v>
+        <v>-6.753537709357972</v>
       </c>
       <c r="E9">
-        <v>1.1702177449279821E-8</v>
+        <v>1.4428236383423609E-11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -2640,7 +2652,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-401.4433662257324</v>
+        <v>-419.20304871843422</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -2651,7 +2663,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-245.4452960540147</v>
+        <v>-256.15193093219727</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -2662,7 +2674,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>311.99614034343551</v>
+        <v>326.10223557247372</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -2673,7 +2685,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.38859297050632968</v>
+        <v>0.38895499039119169</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -2684,7 +2696,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.36866487934065928</v>
+        <v>0.36987115971663631</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2695,7 +2707,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>506.89059210802941</v>
+        <v>528.30386186439466</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -2706,7 +2718,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>535.37604515615362</v>
+        <v>556.78931491251888</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -2717,7 +2729,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.016644546989727E-6</v>
+        <v>1.053719856793302E-6</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -2737,7 +2749,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9AD6D0-AB0B-4834-ACD0-4FE57F7A2CBF}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3046,13 +3058,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-9.2439678561207508</v>
+        <v>-8.9222686023293889</v>
       </c>
       <c r="C2">
-        <v>0.8344435829162351</v>
+        <v>0.82800018004566867</v>
       </c>
       <c r="D2">
-        <v>-11.078002210544531</v>
+        <v>-10.7756843746547</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3063,16 +3075,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>3.6443723477172671</v>
+        <v>2.9185743277765051</v>
       </c>
       <c r="C3">
-        <v>1.1619817183414729</v>
+        <v>0.75150296426339669</v>
       </c>
       <c r="D3">
-        <v>3.1363422420440261</v>
+        <v>3.8836497879116338</v>
       </c>
       <c r="E3">
-        <v>1.710694445186123E-3</v>
+        <v>1.0290009113989031E-4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -3080,16 +3092,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.91117919426635541</v>
+        <v>0.94656135486377702</v>
       </c>
       <c r="C4">
-        <v>0.90862624206650688</v>
+        <v>0.92063837909468371</v>
       </c>
       <c r="D4">
-        <v>1.002809683543854</v>
+        <v>1.028157609282577</v>
       </c>
       <c r="E4">
-        <v>0.31595269572957152</v>
+        <v>0.30387569514037671</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -3097,16 +3109,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.67067888262896003</v>
+        <v>0.44139173249000269</v>
       </c>
       <c r="C5">
-        <v>1.70274925512211</v>
+        <v>1.7044499752326689</v>
       </c>
       <c r="D5">
-        <v>0.39388000353631819</v>
+        <v>0.25896432215897081</v>
       </c>
       <c r="E5">
-        <v>0.69366963433548534</v>
+        <v>0.79566276846224016</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -3114,16 +3126,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.482480495720971</v>
+        <v>1.8704409168759419</v>
       </c>
       <c r="C6">
-        <v>0.9014244554566434</v>
+        <v>0.65021143583864105</v>
       </c>
       <c r="D6">
-        <v>1.6445975996623881</v>
+        <v>2.8766656717802142</v>
       </c>
       <c r="E6">
-        <v>0.1000528221979067</v>
+        <v>4.0190116065643711E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -3131,16 +3143,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2.535256935735823</v>
+        <v>2.7453002702234448</v>
       </c>
       <c r="C7">
-        <v>0.74092185187721038</v>
+        <v>0.55514816281835322</v>
       </c>
       <c r="D7">
-        <v>3.4217602427468692</v>
+        <v>4.9451668114800524</v>
       </c>
       <c r="E7">
-        <v>6.2217151093180156E-4</v>
+        <v>7.6078689614789141E-7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -3148,16 +3160,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-3.1180794658561811E-2</v>
+        <v>-2.0888352142721101E-2</v>
       </c>
       <c r="C8">
-        <v>2.1632317462137361E-2</v>
+        <v>1.4230444794745001E-2</v>
       </c>
       <c r="D8">
-        <v>-1.441398718058617</v>
+        <v>-1.4678636152282969</v>
       </c>
       <c r="E8">
-        <v>0.1494720722399652</v>
+        <v>0.1421412732216196</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -3189,7 +3201,7 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>-39.00172338315145</v>
+        <v>-37.729598455444517</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -3200,7 +3212,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-27.696439279001829</v>
+        <v>-28.641191885508661</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -3211,7 +3223,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>22.610568208299231</v>
+        <v>18.176813139871729</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -3222,7 +3234,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>0.28986627060263298</v>
+        <v>0.24088267413363831</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -3233,7 +3245,7 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.1103870221798834</v>
+        <v>5.5351942650598167E-2</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -3244,7 +3256,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>69.392878558003673</v>
+        <v>71.282383771017322</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -3255,7 +3267,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>80.855981676088362</v>
+        <v>82.745486889102011</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -3266,7 +3278,7 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>9.1768176191614812E-5</v>
+        <v>1.182978350206984E-4</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -3312,16 +3324,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-0.17642635409938229</v>
+        <v>-0.1269627740769981</v>
       </c>
       <c r="C2">
-        <v>0.66429763907101214</v>
+        <v>0.5783775478249773</v>
       </c>
       <c r="D2">
-        <v>-0.26558329237193429</v>
+        <v>-0.21951539190006439</v>
       </c>
       <c r="E2">
-        <v>0.79056015438090355</v>
+        <v>0.82624859123976124</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -3329,13 +3341,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-3.604824408821484</v>
+        <v>-3.2255623081650948</v>
       </c>
       <c r="C3">
-        <v>0.2255847841661659</v>
+        <v>0.21656144723227419</v>
       </c>
       <c r="D3">
-        <v>-15.97990938150406</v>
+        <v>-14.894443814394631</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3346,13 +3358,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-3.1987919143328432</v>
+        <v>-3.110550593875558</v>
       </c>
       <c r="C4">
-        <v>0.36045846465984882</v>
+        <v>0.35780969961802361</v>
       </c>
       <c r="D4">
-        <v>-8.8742316464989202</v>
+        <v>-8.6933098716893298</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -3363,16 +3375,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-8.4769151540964867</v>
+        <v>-8.3521333434421035</v>
       </c>
       <c r="C5">
-        <v>2.1294133574743879</v>
+        <v>2.131109103184869</v>
       </c>
       <c r="D5">
-        <v>-3.9808687798176559</v>
+        <v>-3.919148640001644</v>
       </c>
       <c r="E5">
-        <v>6.8663848155070539E-5</v>
+        <v>8.8862302088266176E-5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -3380,13 +3392,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-2.497283515697148</v>
+        <v>-2.2827141547702832</v>
       </c>
       <c r="C6">
-        <v>0.21262660012990689</v>
+        <v>0.19658230835799059</v>
       </c>
       <c r="D6">
-        <v>-11.74492520771814</v>
+        <v>-11.6120019844985</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -3397,13 +3409,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-3.470494302295112</v>
+        <v>-3.3743528676811998</v>
       </c>
       <c r="C7">
-        <v>0.15428015417550489</v>
+        <v>0.1611658260846392</v>
       </c>
       <c r="D7">
-        <v>-22.49475521230794</v>
+        <v>-20.93714870985799</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -3414,16 +3426,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-1.228136673447641E-2</v>
+        <v>-1.493257175468663E-2</v>
       </c>
       <c r="C8">
-        <v>3.162914823230585E-3</v>
+        <v>3.346676778157435E-3</v>
       </c>
       <c r="D8">
-        <v>-3.8829268003911279</v>
+        <v>-4.4619103500362503</v>
       </c>
       <c r="E8">
-        <v>1.032066446138291E-4</v>
+        <v>8.1232211766035789E-6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -3439,7 +3451,7 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>2843</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -3455,7 +3467,7 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>-2912.6366730344698</v>
+        <v>-3028.8638748948379</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -3466,7 +3478,7 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>-492.42030962700642</v>
+        <v>-535.98964123582937</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -3477,7 +3489,7 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>4840.4327268149273</v>
+        <v>4985.7484673180179</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -3488,7 +3500,7 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>0.83093658258653025</v>
+        <v>0.82303937602529631</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -3499,7 +3511,7 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.82853326188923671</v>
+        <v>0.82072827843586005</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -3510,7 +3522,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>998.84061925401272</v>
+        <v>1085.979282471659</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -3521,7 +3533,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>1040.50892503557</v>
+        <v>1127.94878770167</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -3532,7 +3544,7 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>8.6301317044096173E-4</v>
+        <v>7.0955165228789373E-4</v>
       </c>
       <c r="C19" t="s">
         <v>25</v>
@@ -3555,7 +3567,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -3595,16 +3609,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>7.145444945642474</v>
+        <v>5.0360158157419308</v>
       </c>
       <c r="C3">
-        <v>0.59142170922531201</v>
+        <v>1.0807691329374871</v>
       </c>
       <c r="D3">
-        <v>12.08181038028196</v>
+        <v>4.6596591836910077</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>3.1673337346216361E-6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -3612,16 +3626,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-5.1308057071405981</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.38246492098671042</v>
+        <v>1.9143119566707841E-10</v>
       </c>
       <c r="D4">
-        <v>-13.415101426566849</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -3629,16 +3643,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-7.2999408337098117</v>
+        <v>-11.460938824138101</v>
       </c>
       <c r="C5">
-        <v>1.057029488716559</v>
+        <v>2.724032798041172</v>
       </c>
       <c r="D5">
-        <v>-6.9060900491748569</v>
+        <v>-4.2073424491729901</v>
       </c>
       <c r="E5">
-        <v>4.9820148007029267E-12</v>
+        <v>2.5839142924644069E-5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -3646,16 +3660,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-2.0156123878173542</v>
+        <v>0.77958296852499054</v>
       </c>
       <c r="C6">
-        <v>1.841668111980205</v>
+        <v>4.4074630131912214</v>
       </c>
       <c r="D6">
-        <v>-1.0944493064226</v>
+        <v>0.17687793775960331</v>
       </c>
       <c r="E6">
-        <v>0.27375796910236389</v>
+        <v>0.85960426848705107</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -3663,16 +3677,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>7.3009139830274679</v>
+        <v>5.6453400399000593</v>
       </c>
       <c r="C7">
-        <v>0.8235707936367429</v>
+        <v>0.99898509047521977</v>
       </c>
       <c r="D7">
-        <v>8.8649500922536646</v>
+        <v>5.6510753701184431</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1.5944715325844069E-8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -3680,16 +3694,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-0.39808874693430668</v>
+        <v>-0.70317853903774519</v>
       </c>
       <c r="C8">
-        <v>0.2081131153436358</v>
+        <v>0.37260265109687568</v>
       </c>
       <c r="D8">
-        <v>-1.912847954233849</v>
+        <v>-1.88720755734752</v>
       </c>
       <c r="E8">
-        <v>5.5767520044103902E-2</v>
+        <v>5.9132414228509227E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -3697,16 +3711,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-5.0395826913330458E-2</v>
+        <v>-2.5133286669159961E-2</v>
       </c>
       <c r="C9">
-        <v>2.7334948449183012E-2</v>
+        <v>3.66527703511021E-2</v>
       </c>
       <c r="D9">
-        <v>-1.8436408251150991</v>
+        <v>-0.68571315151364098</v>
       </c>
       <c r="E9">
-        <v>6.5235502183687233E-2</v>
+        <v>0.4928940118028442</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -3722,7 +3736,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -3738,7 +3752,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-27.935843471891669</v>
+        <v>-23.66290446941348</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -3749,7 +3763,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-8.077792609212235</v>
+        <v>-7.4933095139041193</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -3760,7 +3774,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>39.716101725358861</v>
+        <v>32.339189911018707</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -3771,7 +3785,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.7108448643285139</v>
+        <v>0.68333094850676823</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -3782,7 +3796,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.42447441669734082</v>
+        <v>0.34524903593594458</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -3793,7 +3807,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>32.15558521842447</v>
+        <v>30.986619027808239</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -3804,7 +3818,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>39.278559281593793</v>
+        <v>37.167328805726477</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -3815,7 +3829,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.3169262323311311E-4</v>
+        <v>8.3047561910798266E-5</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
mode choice estimation with new segments
</commit_message>
<xml_diff>
--- a/input/estimation_results_mode.xlsx
+++ b/input/estimation_results_mode.xlsx
@@ -5,33 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.arnz\Code\quetzal_germany\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.arnz\Code\quetzal_germany\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E7974E-3849-41FF-9568-E253414C2581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26D9A25-6B9F-49C3-B38A-6BF5FAAB2180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="-10700" windowWidth="19380" windowHeight="20970" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36620" yWindow="-8920" windowWidth="28800" windowHeight="15370" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leisure_no_car" sheetId="1" r:id="rId1"/>
     <sheet name="leisure_car" sheetId="2" r:id="rId2"/>
     <sheet name="commuting_no_car" sheetId="3" r:id="rId3"/>
     <sheet name="commuting_car" sheetId="4" r:id="rId4"/>
-    <sheet name="buy-execute_no_car" sheetId="5" r:id="rId5"/>
-    <sheet name="buy-execute_car" sheetId="13" r:id="rId6"/>
-    <sheet name="business_no_car" sheetId="7" r:id="rId7"/>
-    <sheet name="business_car" sheetId="8" r:id="rId8"/>
-    <sheet name="accompany_no_car" sheetId="9" r:id="rId9"/>
-    <sheet name="accompany_car" sheetId="10" r:id="rId10"/>
-    <sheet name="education_no_car" sheetId="11" r:id="rId11"/>
-    <sheet name="education_car" sheetId="12" r:id="rId12"/>
+    <sheet name="errands_no_car" sheetId="5" r:id="rId5"/>
+    <sheet name="errands_car" sheetId="6" r:id="rId6"/>
+    <sheet name="shopping_no_car" sheetId="7" r:id="rId7"/>
+    <sheet name="shopping_car" sheetId="8" r:id="rId8"/>
+    <sheet name="business_no_car" sheetId="9" r:id="rId9"/>
+    <sheet name="business_car" sheetId="10" r:id="rId10"/>
+    <sheet name="accompany_no_car" sheetId="11" r:id="rId11"/>
+    <sheet name="accompany_car" sheetId="12" r:id="rId12"/>
+    <sheet name="education_no_car" sheetId="13" r:id="rId13"/>
+    <sheet name="education_car" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="27">
   <si>
     <t>Value</t>
   </si>
@@ -499,16 +501,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-5.0532471948770334</v>
+        <v>-6.2322460950308631</v>
       </c>
       <c r="C2">
-        <v>0.8423170926111595</v>
+        <v>0.84584228218210589</v>
       </c>
       <c r="D2">
-        <v>-5.9992219547772763</v>
+        <v>-7.3680947693379668</v>
       </c>
       <c r="E2">
-        <v>1.9826520425425538E-9</v>
+        <v>1.7297274723659939E-13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -516,13 +518,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2.3946479373023748</v>
+        <v>2.605308896412037</v>
       </c>
       <c r="C3">
-        <v>0.25364665151762811</v>
+        <v>0.26015228238734178</v>
       </c>
       <c r="D3">
-        <v>9.4408813322574101</v>
+        <v>10.014553293570501</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -533,16 +535,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.1746574554607187</v>
+        <v>0.41281459840186269</v>
       </c>
       <c r="C4">
-        <v>0.39235288652958328</v>
+        <v>0.39403876662571202</v>
       </c>
       <c r="D4">
-        <v>0.44515399645861808</v>
+        <v>1.0476497069994779</v>
       </c>
       <c r="E4">
-        <v>0.65620846945821842</v>
+        <v>0.29480002695773599</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -550,16 +552,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-1.2861372537428011</v>
+        <v>-1.039213137002412</v>
       </c>
       <c r="C5">
-        <v>0.42401948097833952</v>
+        <v>0.42254482986726338</v>
       </c>
       <c r="D5">
-        <v>-3.0332032169260201</v>
+        <v>-2.459415104733067</v>
       </c>
       <c r="E5">
-        <v>2.4197259197851211E-3</v>
+        <v>1.391636066276569E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -567,16 +569,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.609563568270123</v>
+        <v>1.850354772001247</v>
       </c>
       <c r="C6">
-        <v>0.21656942750414851</v>
+        <v>0.2172169122843895</v>
       </c>
       <c r="D6">
-        <v>7.4320904239324879</v>
+        <v>8.518465493969849</v>
       </c>
       <c r="E6">
-        <v>1.068034549689401E-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -584,13 +586,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2.1605154875823098</v>
+        <v>2.4029809651769609</v>
       </c>
       <c r="C7">
-        <v>0.20660568867638321</v>
+        <v>0.20610536417318151</v>
       </c>
       <c r="D7">
-        <v>10.457192642775841</v>
+        <v>11.65899283998178</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -601,16 +603,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-6.3723847274516507E-2</v>
+        <v>-6.3523708043630556E-2</v>
       </c>
       <c r="C8">
-        <v>1.5931690302559001E-2</v>
+        <v>1.60095212367613E-2</v>
       </c>
       <c r="D8">
-        <v>-3.9998170981443799</v>
+        <v>-3.967870563035107</v>
       </c>
       <c r="E8">
-        <v>6.3391457171713128E-5</v>
+        <v>7.251769995386681E-5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -618,16 +620,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-1.3692568852585451E-2</v>
+        <v>-1.354420375276822E-2</v>
       </c>
       <c r="C9">
-        <v>4.491265495140266E-3</v>
+        <v>4.5193027908131964E-3</v>
       </c>
       <c r="D9">
-        <v>-3.0487106289755901</v>
+        <v>-2.9969675367405721</v>
       </c>
       <c r="E9">
-        <v>2.2982573959966501E-3</v>
+        <v>2.7267974919675808E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -670,7 +672,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-351.7223271678256</v>
+        <v>-351.90548911859162</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -681,7 +683,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>312.72998473334968</v>
+        <v>312.3636608318177</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -692,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.30775220391237751</v>
+        <v>0.30739171085592049</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -703,7 +705,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.29200687886208998</v>
+        <v>0.29164638580563301</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -714,7 +716,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>719.44465433565119</v>
+        <v>719.81097823718324</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -725,7 +727,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>751.07060100995352</v>
+        <v>751.43692491148556</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -736,7 +738,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.111233066012662E-3</v>
+        <v>1.358565451940017E-3</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -757,11 +759,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -784,16 +784,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-9.8137289607975589E-2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.59014577284245728</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-0.16629330264502951</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.86792613638186888</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -801,16 +801,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-2.46396062168012</v>
+        <v>-3.2371352921127028</v>
       </c>
       <c r="C3">
-        <v>0.31507374511365782</v>
+        <v>0.21683110013337539</v>
       </c>
       <c r="D3">
-        <v>-7.820266397605697</v>
+        <v>-14.929294230032051</v>
       </c>
       <c r="E3">
-        <v>5.3290705182007514E-15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -818,16 +818,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-4.7096472146805333</v>
+        <v>-3.1230664419903489</v>
       </c>
       <c r="C4">
-        <v>1.3027537243626639</v>
+        <v>0.35844817855916139</v>
       </c>
       <c r="D4">
-        <v>-3.6151477647738819</v>
+        <v>-8.712741837729526</v>
       </c>
       <c r="E4">
-        <v>3.0017635771706352E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -835,16 +835,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-5.2843699536352764</v>
+        <v>-8.3565125163069052</v>
       </c>
       <c r="C5">
-        <v>0.35106059290572689</v>
+        <v>2.1294077622515348</v>
       </c>
       <c r="D5">
-        <v>-15.05258653469639</v>
+        <v>-3.9243364584484861</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>8.6969116301016669E-5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -852,16 +852,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-4.4617519202945592</v>
+        <v>-2.2855286078873229</v>
       </c>
       <c r="C6">
-        <v>2.1435383185895018</v>
+        <v>0.19665630917504201</v>
       </c>
       <c r="D6">
-        <v>-2.0814892281610788</v>
+        <v>-11.62194397665114</v>
       </c>
       <c r="E6">
-        <v>3.7389149047711179E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -869,13 +869,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-3.818045990882974</v>
+        <v>-3.3781030845446329</v>
       </c>
       <c r="C7">
-        <v>0.22365305165472429</v>
+        <v>0.16126167794295901</v>
       </c>
       <c r="D7">
-        <v>-17.07128949341266</v>
+        <v>-20.947959413764291</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -883,68 +883,62 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>-0.21722483227643821</v>
+        <v>-1.469878873562006E-2</v>
       </c>
       <c r="C8">
-        <v>3.9559756839046979E-2</v>
+        <v>3.324686320459987E-3</v>
       </c>
       <c r="D8">
-        <v>-5.4910558009807851</v>
+        <v>-4.4211054273494304</v>
       </c>
       <c r="E8">
-        <v>3.9953808705917033E-8</v>
+        <v>9.819724494875004E-6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>-4.1132003975000157E-2</v>
-      </c>
-      <c r="C9">
-        <v>8.5269513949378737E-3</v>
-      </c>
-      <c r="D9">
-        <v>-4.8237643291151713</v>
-      </c>
-      <c r="E9">
-        <v>1.40873859333368E-6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>5246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-3028.8638748948379</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>-6437.880550479701</v>
+        <v>-536.23209466425476</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -952,10 +946,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>-439.06028147952469</v>
+        <v>4985.2635604611669</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -963,21 +957,21 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>11997.640538000351</v>
+        <v>0.82295932837758423</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>0.93180049271855325</v>
+        <v>0.82064823078814797</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -985,21 +979,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17">
-        <v>0.93055784773045946</v>
+        <v>1086.46418932851</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>894.12056295904949</v>
+        <v>1128.433694558521</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1007,31 +1001,20 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>946.64233224246402</v>
+        <v>9.5683279990377984E-4</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20">
-        <v>1.133524761551212E-4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
         <v>8</v>
       </c>
     </row>
@@ -1044,9 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1074,8 +1055,8 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1086,16 +1067,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.86045471497878</v>
+        <v>5.6077739629177472</v>
       </c>
       <c r="C3">
-        <v>0.55770510369216619</v>
+        <v>1.5014102412551209</v>
       </c>
       <c r="D3">
-        <v>3.3359112238027619</v>
+        <v>3.7350044703503991</v>
       </c>
       <c r="E3">
-        <v>8.5020308899474983E-4</v>
+        <v>1.8771185275712199E-4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1103,16 +1084,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.95081138431308654</v>
-      </c>
-      <c r="C4">
-        <v>0.85166473594446135</v>
+        <v>0</v>
+      </c>
+      <c r="C4" t="e">
+        <v>#NULL!</v>
       </c>
       <c r="D4">
-        <v>1.1164151152256829</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.26424448641742432</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1120,16 +1101,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-4.1145883589905523</v>
+        <v>-8.305614117497587</v>
       </c>
       <c r="C5">
-        <v>1.8437366401560471</v>
+        <v>3.171546177271777</v>
       </c>
       <c r="D5">
-        <v>-2.2316573144862542</v>
+        <v>-2.6187902219485348</v>
       </c>
       <c r="E5">
-        <v>2.5637620462940051E-2</v>
+        <v>8.8242193985987871E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1137,16 +1118,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>6.8728850869433034E-2</v>
+        <v>-3.6246938471859398</v>
       </c>
       <c r="C6">
-        <v>1.3700185015651249</v>
+        <v>6.375832692986604</v>
       </c>
       <c r="D6">
-        <v>5.0166366943888999E-2</v>
+        <v>-0.56850516971267018</v>
       </c>
       <c r="E6">
-        <v>0.95998981308267251</v>
+        <v>0.5696919963607896</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1154,16 +1135,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.234593408829292</v>
+        <v>6.3225340017444358</v>
       </c>
       <c r="C7">
-        <v>0.47177831564464912</v>
+        <v>1.9381650344222541</v>
       </c>
       <c r="D7">
-        <v>2.6168930785687219</v>
+        <v>3.2621236527616522</v>
       </c>
       <c r="E7">
-        <v>8.8734131505059377E-3</v>
+        <v>1.1058089662070449E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1171,16 +1152,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-8.385236116477586E-2</v>
+        <v>-0.29087329773142079</v>
       </c>
       <c r="C8">
-        <v>5.6163160810944801E-2</v>
+        <v>0.57898961210067035</v>
       </c>
       <c r="D8">
-        <v>-1.4930135689306701</v>
+        <v>-0.5023808573630264</v>
       </c>
       <c r="E8">
-        <v>0.13543363509348261</v>
+        <v>0.61539964182549123</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1188,16 +1169,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-3.4084377185844963E-2</v>
+        <v>-3.2002141735101713E-2</v>
       </c>
       <c r="C9">
-        <v>3.018770220858499E-2</v>
+        <v>3.8398266555244663E-2</v>
       </c>
       <c r="D9">
-        <v>-1.129081536260544</v>
+        <v>-0.83342673005978873</v>
       </c>
       <c r="E9">
-        <v>0.25886343940846679</v>
+        <v>0.40460410468393748</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1213,7 +1194,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1229,7 +1210,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-168.70704678905281</v>
+        <v>-23.66290446941348</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1240,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-104.2569847307753</v>
+        <v>-8.2272028289314605</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1251,7 +1232,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>128.90012411655511</v>
+        <v>30.871403280964032</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1262,7 +1243,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.38202353301142389</v>
+        <v>0.65231644156084512</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1273,7 +1254,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.33460405556657841</v>
+        <v>0.31423452899002141</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -1284,7 +1265,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>224.51396946155049</v>
+        <v>32.454405657862921</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1295,7 +1276,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>242.3868214983286</v>
+        <v>38.635115435781167</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1306,7 +1287,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>7.4054413197065249E-4</v>
+        <v>9.2582828278994534E-5</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1329,9 +1310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1359,8 +1338,8 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1371,13 +1350,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.87468872115164675</v>
+        <v>-3.0305672426493131</v>
       </c>
       <c r="C3">
-        <v>9.5767107594211184E-2</v>
+        <v>0.2494397279027176</v>
       </c>
       <c r="D3">
-        <v>9.1334983704208579</v>
+        <v>-12.149497067408779</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1388,16 +1367,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-0.81426292023067048</v>
+        <v>-5.0105766913418659</v>
       </c>
       <c r="C4">
-        <v>0.22143532529444729</v>
+        <v>1.3209235861057269</v>
       </c>
       <c r="D4">
-        <v>-3.6772042543254</v>
+        <v>-3.7932373560788379</v>
       </c>
       <c r="E4">
-        <v>2.3580422134528159E-4</v>
+        <v>1.486958972936048E-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1405,13 +1384,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-2.727770620754479</v>
+        <v>-5.8099704603137647</v>
       </c>
       <c r="C5">
-        <v>0.18043216670388659</v>
+        <v>0.37943165717654281</v>
       </c>
       <c r="D5">
-        <v>-15.117984063402149</v>
+        <v>-15.312297617830261</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1422,16 +1401,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-2.628210351262092</v>
+        <v>-4.6346904056303568</v>
       </c>
       <c r="C6">
-        <v>0.51809890491310606</v>
+        <v>2.4323573866832868</v>
       </c>
       <c r="D6">
-        <v>-5.0727965767518608</v>
+        <v>-1.905431508956883</v>
       </c>
       <c r="E6">
-        <v>3.9201149504286548E-7</v>
+        <v>5.6724002646187488E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1439,16 +1418,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-0.29332225431651282</v>
+        <v>-4.2151209875194358</v>
       </c>
       <c r="C7">
-        <v>7.0749046755809258E-2</v>
+        <v>0.21100629218076319</v>
       </c>
       <c r="D7">
-        <v>-4.1459534476685773</v>
+        <v>-19.976281010181719</v>
       </c>
       <c r="E7">
-        <v>3.3840258093720272E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1456,16 +1435,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-3.3921924421893443E-2</v>
+        <v>-0.24889162926273181</v>
       </c>
       <c r="C8">
-        <v>8.8236872345383993E-3</v>
+        <v>4.6441721412528447E-2</v>
       </c>
       <c r="D8">
-        <v>-3.8444160043562592</v>
+        <v>-5.3592248885845342</v>
       </c>
       <c r="E8">
-        <v>1.20839865210165E-4</v>
+        <v>8.3579762444330186E-8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1473,16 +1452,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-3.972621361058884E-2</v>
+        <v>-4.0295593872481827E-2</v>
       </c>
       <c r="C9">
-        <v>4.4745437749785909E-3</v>
+        <v>8.1105997686659864E-3</v>
       </c>
       <c r="D9">
-        <v>-8.8782713072862744</v>
+        <v>-4.9682631398182728</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>6.755525070456514E-7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1498,7 +1477,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>2589</v>
+        <v>5246</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1514,7 +1493,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-3334.025990199621</v>
+        <v>-6437.880550479701</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1525,7 +1504,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-2636.2555675374701</v>
+        <v>-429.68639045220942</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1536,7 +1515,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>1395.5408453243019</v>
+        <v>12016.388320054981</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1547,7 +1526,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.20928763744291409</v>
+        <v>0.93325654505655709</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1558,7 +1537,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.20688813605224829</v>
+        <v>0.9320139000684633</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -1569,7 +1548,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>5288.5111350749394</v>
+        <v>875.37278090441873</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1580,7 +1559,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>5335.3833509129518</v>
+        <v>927.89455018783326</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1591,7 +1570,573 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>4.6615943184417328E-4</v>
+        <v>1.788000370761508E-3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1.7201004212116791</v>
+      </c>
+      <c r="C3">
+        <v>0.55629978355909615</v>
+      </c>
+      <c r="D3">
+        <v>3.092038631053954</v>
+      </c>
+      <c r="E3">
+        <v>1.9878697761355202E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.82010096047164549</v>
+      </c>
+      <c r="C4">
+        <v>0.87046482759563926</v>
+      </c>
+      <c r="D4">
+        <v>0.94214141051154621</v>
+      </c>
+      <c r="E4">
+        <v>0.34612024564216531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>-4.3156357070738061</v>
+      </c>
+      <c r="C5">
+        <v>1.841089291721183</v>
+      </c>
+      <c r="D5">
+        <v>-2.3440664863349672</v>
+      </c>
+      <c r="E5">
+        <v>1.907477077302322E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.61148906156012739</v>
+      </c>
+      <c r="C6">
+        <v>1.303357309282525</v>
+      </c>
+      <c r="D6">
+        <v>0.46916456232308329</v>
+      </c>
+      <c r="E6">
+        <v>0.63895201368665422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1.1639452638303229</v>
+      </c>
+      <c r="C7">
+        <v>0.47328902730304578</v>
+      </c>
+      <c r="D7">
+        <v>2.4592694879550878</v>
+      </c>
+      <c r="E7">
+        <v>1.3922006986963661E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>-0.1215737650139687</v>
+      </c>
+      <c r="C8">
+        <v>5.474120561607973E-2</v>
+      </c>
+      <c r="D8">
+        <v>-2.220882124274179</v>
+      </c>
+      <c r="E8">
+        <v>2.6358946273758791E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>-3.2150463993493333E-2</v>
+      </c>
+      <c r="C9">
+        <v>3.0388999615964779E-2</v>
+      </c>
+      <c r="D9">
+        <v>-1.0579638816607571</v>
+      </c>
+      <c r="E9">
+        <v>0.29007190920770309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>-168.70704678905281</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>-102.9868379200805</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>131.44041773794461</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0.38955224526659649</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0.34213276782175089</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>221.97367584016109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>239.84652787693909</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>8.2144612919503074E-4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.80583666785138808</v>
+      </c>
+      <c r="C3">
+        <v>8.931323381641823E-2</v>
+      </c>
+      <c r="D3">
+        <v>9.0225897486566335</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>-0.96209941355823803</v>
+      </c>
+      <c r="C4">
+        <v>0.23144550548851781</v>
+      </c>
+      <c r="D4">
+        <v>-4.1569155189577378</v>
+      </c>
+      <c r="E4">
+        <v>3.2257320551565272E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>-2.9388316777306338</v>
+      </c>
+      <c r="C5">
+        <v>0.1817692277611459</v>
+      </c>
+      <c r="D5">
+        <v>-16.167927398538598</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>-2.1342225622157902</v>
+      </c>
+      <c r="C6">
+        <v>0.50349253034270158</v>
+      </c>
+      <c r="D6">
+        <v>-4.2388365935898484</v>
+      </c>
+      <c r="E6">
+        <v>2.2468111965157082E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>-0.35476750527879541</v>
+      </c>
+      <c r="C7">
+        <v>6.6489118007188999E-2</v>
+      </c>
+      <c r="D7">
+        <v>-5.3357228357343658</v>
+      </c>
+      <c r="E7">
+        <v>9.5164675251169228E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>-7.4143809381882239E-2</v>
+      </c>
+      <c r="C8">
+        <v>8.7248795838749255E-3</v>
+      </c>
+      <c r="D8">
+        <v>-8.4979750917035837</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>-3.953679452608725E-2</v>
+      </c>
+      <c r="C9">
+        <v>4.512025454640114E-3</v>
+      </c>
+      <c r="D9">
+        <v>-8.7625380050611366</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>2589</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>-3334.025990199621</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>-2605.3037438758638</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>1457.444492647513</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0.21857125543287231</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0.21617175404220651</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>5226.6074877517294</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>5273.4797035897409</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>2.0930473914765419E-4</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1637,16 +2182,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.12443955808591391</v>
+        <v>0.99783421800255256</v>
       </c>
       <c r="C2">
-        <v>0.59969315623044994</v>
+        <v>0.56152008721682167</v>
       </c>
       <c r="D2">
-        <v>0.20750538303307611</v>
+        <v>1.7770231924352431</v>
       </c>
       <c r="E2">
-        <v>0.83561518911108346</v>
+        <v>7.5564424033489619E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1654,13 +2199,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-2.470159158229102</v>
+        <v>-2.542086270756382</v>
       </c>
       <c r="C3">
-        <v>8.1628130977825147E-2</v>
+        <v>6.8802129648912191E-2</v>
       </c>
       <c r="D3">
-        <v>-30.261126019167801</v>
+        <v>-36.947784664926793</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1671,13 +2216,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-2.8858598474839061</v>
+        <v>-2.891335453612228</v>
       </c>
       <c r="C4">
-        <v>0.18851576250138141</v>
+        <v>0.18874915664174149</v>
       </c>
       <c r="D4">
-        <v>-15.30832122042187</v>
+        <v>-15.31840197357902</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1688,13 +2233,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-3.5838579737122669</v>
+        <v>-3.6193953774530989</v>
       </c>
       <c r="C5">
-        <v>8.2243930221597594E-2</v>
+        <v>8.5205827532901457E-2</v>
       </c>
       <c r="D5">
-        <v>-43.57595708347035</v>
+        <v>-42.478260962320952</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1705,13 +2250,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-2.5965508934771209</v>
+        <v>-2.6658625003834522</v>
       </c>
       <c r="C6">
-        <v>0.22726057369729799</v>
+        <v>0.1773410537247494</v>
       </c>
       <c r="D6">
-        <v>-11.42543491479355</v>
+        <v>-15.032404761286299</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1722,13 +2267,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-2.4594236893706301</v>
+        <v>-2.5040178430845801</v>
       </c>
       <c r="C7">
-        <v>5.9630816451050207E-2</v>
+        <v>4.9936880685116543E-2</v>
       </c>
       <c r="D7">
-        <v>-41.244172656759183</v>
+        <v>-50.143657527869799</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1739,16 +2284,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-2.6894443092045878E-2</v>
+        <v>-2.385279439734329E-2</v>
       </c>
       <c r="C8">
-        <v>1.15425278910396E-2</v>
+        <v>7.9509507333823254E-3</v>
       </c>
       <c r="D8">
-        <v>-2.330030591732327</v>
+        <v>-2.999992730076487</v>
       </c>
       <c r="E8">
-        <v>1.9804534312010121E-2</v>
+        <v>2.699860502360929E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1756,13 +2301,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-1.8364013070772858E-2</v>
+        <v>-1.8454677803358421E-2</v>
       </c>
       <c r="C9">
-        <v>1.5508245659285849E-3</v>
+        <v>1.537553778213448E-3</v>
       </c>
       <c r="D9">
-        <v>-11.84145097661454</v>
+        <v>-12.002622649597161</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1781,7 +2326,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>17197</v>
+        <v>17199</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1797,7 +2342,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-19159.529429758459</v>
+        <v>-19169.03376525121</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -1808,7 +2353,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-5564.1730354486908</v>
+        <v>-5576.7282185917957</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -1819,7 +2364,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>27190.712788619541</v>
+        <v>27184.611093318821</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1830,7 +2375,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.70958717666591264</v>
+        <v>0.70907619617734485</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1841,7 +2386,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.70916962987650267</v>
+        <v>0.70865885641478976</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -1852,7 +2397,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>11144.34607089738</v>
+        <v>11169.45643718359</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -1863,7 +2408,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>11206.365992729259</v>
+        <v>11231.4772893562</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1874,7 +2419,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.9957920849218599E-2</v>
+        <v>1.3512697280706001E-2</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -1898,7 +2443,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1927,8 +2472,8 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1939,16 +2484,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>1.3424267654694899</v>
+        <v>1.3254180727833831</v>
       </c>
       <c r="C3">
-        <v>0.20680535299576791</v>
+        <v>0.2088525836338414</v>
       </c>
       <c r="D3">
-        <v>6.4912573394411188</v>
+        <v>6.3461894975026727</v>
       </c>
       <c r="E3">
-        <v>8.5123019744060002E-11</v>
+        <v>2.2071344751850569E-10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1956,16 +2501,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-0.9845398117062335</v>
+        <v>-0.9899541260298157</v>
       </c>
       <c r="C4">
-        <v>0.3392098615863407</v>
+        <v>0.33958851528922229</v>
       </c>
       <c r="D4">
-        <v>-2.902450439093835</v>
+        <v>-2.915157849748502</v>
       </c>
       <c r="E4">
-        <v>3.702557402778472E-3</v>
+        <v>3.5550868239939688E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1973,16 +2518,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-2.8942148064322888</v>
+        <v>-2.905413147496672</v>
       </c>
       <c r="C5">
-        <v>0.55861222683102474</v>
+        <v>0.5578949088408075</v>
       </c>
       <c r="D5">
-        <v>-5.1810803047598943</v>
+        <v>-5.2078144135309117</v>
       </c>
       <c r="E5">
-        <v>2.206044844577093E-7</v>
+        <v>1.910778903990717E-7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1990,16 +2535,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.74071104863284765</v>
+        <v>0.78185006474226115</v>
       </c>
       <c r="C6">
-        <v>0.47040726699080188</v>
+        <v>0.47407005081925019</v>
       </c>
       <c r="D6">
-        <v>1.574616509160627</v>
+        <v>1.6492289765850641</v>
       </c>
       <c r="E6">
-        <v>0.1153449898155807</v>
+        <v>9.9100733707297328E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2007,13 +2552,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.7956168040361971</v>
+        <v>1.7880991360008429</v>
       </c>
       <c r="C7">
-        <v>0.19571380491900761</v>
+        <v>0.1965899426245675</v>
       </c>
       <c r="D7">
-        <v>9.1747069389370779</v>
+        <v>9.0955778923829236</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2024,16 +2569,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-4.101186323576636E-2</v>
+        <v>-4.3986903859831623E-2</v>
       </c>
       <c r="C8">
-        <v>2.7278725849460759E-2</v>
+        <v>2.7916563335977859E-2</v>
       </c>
       <c r="D8">
-        <v>-1.503437640822842</v>
+        <v>-1.575656119646464</v>
       </c>
       <c r="E8">
-        <v>0.13272622623234051</v>
+        <v>0.11510507524628449</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2044,13 +2589,13 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>2.5004850056551879E-3</v>
+        <v>2.4988815276966989E-3</v>
       </c>
       <c r="D9">
-        <v>1.2685481246163619</v>
+        <v>1.2728324137879921</v>
       </c>
       <c r="E9">
-        <v>0.2046022762196282</v>
+        <v>0.2030775164218421</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -2093,7 +2638,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-404.49857100579987</v>
+        <v>-404.3554694398839</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -2104,7 +2649,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>410.67316403475962</v>
+        <v>410.95936716659162</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -2115,7 +2660,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.33670833994965688</v>
+        <v>0.33694299609436518</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -2126,7 +2671,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.32359004074971559</v>
+        <v>0.32382469689442389</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2137,7 +2682,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>824.99714201159986</v>
+        <v>824.71093887976781</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -2148,7 +2693,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>855.88343179932679</v>
+        <v>855.59722866749473</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -2159,7 +2704,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>9.3213283476952999E-7</v>
+        <v>9.4085929846914563E-7</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -2182,9 +2727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -2212,8 +2755,8 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2224,13 +2767,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-1.818434104221158</v>
+        <v>-2.7295821863411671</v>
       </c>
       <c r="C3">
-        <v>8.4450303317423897E-2</v>
+        <v>8.6747223014969815E-2</v>
       </c>
       <c r="D3">
-        <v>-21.532594114981421</v>
+        <v>-31.46593160532791</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2241,13 +2784,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-5.2444468548668262</v>
+        <v>-6.2902385631058202</v>
       </c>
       <c r="C4">
-        <v>0.43483331359388933</v>
+        <v>0.5617180998289808</v>
       </c>
       <c r="D4">
-        <v>-12.060821217954921</v>
+        <v>-11.198212350680761</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2258,13 +2801,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-6.2916545775286998</v>
+        <v>-7.1941117040429896</v>
       </c>
       <c r="C5">
-        <v>0.2458395768574953</v>
+        <v>0.25667720340185629</v>
       </c>
       <c r="D5">
-        <v>-25.592521179678709</v>
+        <v>-28.02785603355596</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2275,16 +2818,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.30254715379359809</v>
+        <v>0.75818432769260669</v>
       </c>
       <c r="C6">
-        <v>0.18117736288328801</v>
+        <v>0.21387610860161591</v>
       </c>
       <c r="D6">
-        <v>1.669894897347054</v>
+        <v>3.5449697147093051</v>
       </c>
       <c r="E6">
-        <v>9.4940160089753922E-2</v>
+        <v>3.9265819899236831E-4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2292,13 +2835,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-1.905261796000334</v>
+        <v>-2.56939061608771</v>
       </c>
       <c r="C7">
-        <v>4.0901425394536867E-2</v>
+        <v>5.008244034503187E-2</v>
       </c>
       <c r="D7">
-        <v>-46.581794585936763</v>
+        <v>-51.30322321329519</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2309,13 +2852,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-0.22834182345483409</v>
+        <v>-0.28115749530568979</v>
       </c>
       <c r="C8">
-        <v>9.1512028005063459E-3</v>
+        <v>1.3597323718745811E-2</v>
       </c>
       <c r="D8">
-        <v>-24.95211049657863</v>
+        <v>-20.67741425601826</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2326,13 +2869,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-1.380099840461871E-2</v>
+        <v>-1.364896613508457E-2</v>
       </c>
       <c r="C9">
-        <v>1.2488932629084639E-3</v>
+        <v>1.233398974145715E-3</v>
       </c>
       <c r="D9">
-        <v>-11.05058279558534</v>
+        <v>-11.066140333494451</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2378,7 +2921,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-4914.450725121379</v>
+        <v>-4798.8974302239994</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -2389,7 +2932,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>25102.833744105461</v>
+        <v>25333.94033390022</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -2400,7 +2943,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.71862544486959745</v>
+        <v>0.72524139419215361</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -2411,7 +2954,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.71816740864806472</v>
+        <v>0.72478335797062088</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2422,7 +2965,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>9844.9014502427581</v>
+        <v>9613.7948604479989</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -2433,7 +2976,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>9905.7733082806481</v>
+        <v>9674.6667184858889</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -2444,7 +2987,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.018034693309005E-2</v>
+        <v>1.7783078747774791E-2</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -2468,7 +3011,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2497,8 +3040,8 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2509,16 +3052,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2.046759948579826</v>
+        <v>2.6080617064640079</v>
       </c>
       <c r="C3">
-        <v>0.26758952740363617</v>
+        <v>0.49665687170469908</v>
       </c>
       <c r="D3">
-        <v>7.648879118847062</v>
+        <v>5.2512345143081047</v>
       </c>
       <c r="E3">
-        <v>2.0206059048177849E-14</v>
+        <v>1.510831753037678E-7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2526,16 +3069,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1.426902315030546</v>
+        <v>0.80622603071315213</v>
       </c>
       <c r="C4">
-        <v>0.44024364321102238</v>
+        <v>0.66983548401701032</v>
       </c>
       <c r="D4">
-        <v>3.2411650617442018</v>
+        <v>1.2036179777729989</v>
       </c>
       <c r="E4">
-        <v>1.190422332844054E-3</v>
+        <v>0.228737267647287</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -2543,16 +3086,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-1.38646927575381</v>
+        <v>-1.348989232800222</v>
       </c>
       <c r="C5">
-        <v>0.3799564701572134</v>
+        <v>0.76679327582204648</v>
       </c>
       <c r="D5">
-        <v>-3.6490213607367559</v>
+        <v>-1.759260644733782</v>
       </c>
       <c r="E5">
-        <v>2.632412173892984E-4</v>
+        <v>7.8533247860401501E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -2560,16 +3103,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-3.3199784516519322</v>
+        <v>-4.0061229114840886</v>
       </c>
       <c r="C6">
-        <v>0.89476720981145863</v>
+        <v>1.595770193575937</v>
       </c>
       <c r="D6">
-        <v>-3.7104382181724151</v>
+        <v>-2.51046355397003</v>
       </c>
       <c r="E6">
-        <v>2.0690078701512959E-4</v>
+        <v>1.205727677319168E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2577,16 +3120,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.2327854637953739</v>
+        <v>1.940824407107141</v>
       </c>
       <c r="C7">
-        <v>0.25037184609388841</v>
+        <v>0.4838869154849581</v>
       </c>
       <c r="D7">
-        <v>4.9238182448560313</v>
+        <v>4.010904913934322</v>
       </c>
       <c r="E7">
-        <v>8.487167080239999E-7</v>
+        <v>6.0486468716147712E-5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2597,13 +3140,13 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>3.1191018598676509E-2</v>
+        <v>4.0810807650271577E-2</v>
       </c>
       <c r="D8">
-        <v>0.29386688574690378</v>
+        <v>2.818435391200584</v>
       </c>
       <c r="E8">
-        <v>0.76885962276917574</v>
+        <v>4.8258322082257443E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2611,16 +3154,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-8.3397779283480508E-2</v>
+        <v>-7.0872474034295016E-2</v>
       </c>
       <c r="C9">
-        <v>1.234875451541808E-2</v>
+        <v>1.3785984053590871E-2</v>
       </c>
       <c r="D9">
-        <v>-6.753537709357972</v>
+        <v>-5.1409078785228006</v>
       </c>
       <c r="E9">
-        <v>1.4428236383423609E-11</v>
+        <v>2.7341409181147469E-7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -2636,7 +3179,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>260</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2652,7 +3195,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-419.20304871843422</v>
+        <v>-267.80717898397768</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -2663,7 +3206,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-256.15193093219727</v>
+        <v>-158.40800348739469</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -2674,7 +3217,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>326.10223557247372</v>
+        <v>218.798350993166</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -2685,7 +3228,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.38895499039119169</v>
+        <v>0.40849978671829451</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -2696,7 +3239,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.36987115971663631</v>
+        <v>0.37862754792936099</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2707,7 +3250,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>528.30386186439466</v>
+        <v>332.81600697478939</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -2718,7 +3261,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>556.78931491251888</v>
+        <v>357.61493839738301</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -2729,7 +3272,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>1.053719856793302E-6</v>
+        <v>2.0801912899156911E-7</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -2749,7 +3292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9AD6D0-AB0B-4834-ACD0-4FE57F7A2CBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2775,16 +3318,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3.705243274177338</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2.3426045368736488</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.5816768113674931</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.1137233689900685</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -2792,13 +3335,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>-3.201578239883049</v>
+        <v>-3.0636132427031888</v>
       </c>
       <c r="C3">
-        <v>9.8878487562078454E-2</v>
+        <v>0.118284376731653</v>
       </c>
       <c r="D3">
-        <v>-32.378915968683437</v>
+        <v>-25.90040483244449</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2809,13 +3352,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>-4.4401702711798574</v>
+        <v>-3.879255016765657</v>
       </c>
       <c r="C4">
-        <v>0.34238927236922628</v>
+        <v>0.35613279560295608</v>
       </c>
       <c r="D4">
-        <v>-12.96819330949031</v>
+        <v>-10.892720537567531</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -2826,13 +3369,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>-4.9767316214201109</v>
+        <v>-5.2354773179624541</v>
       </c>
       <c r="C5">
-        <v>0.1185213287507077</v>
+        <v>0.21523191114173479</v>
       </c>
       <c r="D5">
-        <v>-41.990177412606812</v>
+        <v>-24.324819169192711</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2843,16 +3386,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>-2.8292310829564991</v>
+        <v>-2.9775803301825419</v>
       </c>
       <c r="C6">
-        <v>0.38435065041314792</v>
+        <v>0.41920828728169568</v>
       </c>
       <c r="D6">
-        <v>-7.3610675041535361</v>
+        <v>-7.102866094299551</v>
       </c>
       <c r="E6">
-        <v>1.8252066524837571E-13</v>
+        <v>1.2219114609024471E-12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -2860,13 +3403,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>-3.229816588592147</v>
+        <v>-3.0090298005717999</v>
       </c>
       <c r="C7">
-        <v>6.3790612399695773E-2</v>
+        <v>8.5064720681338454E-2</v>
       </c>
       <c r="D7">
-        <v>-50.631534438875377</v>
+        <v>-35.373416575879297</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2877,16 +3420,16 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>-0.1188072839579022</v>
+        <v>-9.7006552513896185E-2</v>
       </c>
       <c r="C8">
-        <v>1.3085566604374099E-2</v>
+        <v>1.48708630892623E-2</v>
       </c>
       <c r="D8">
-        <v>-9.0792617201756176</v>
+        <v>-6.523263103937861</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>6.8794081542478125E-11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -2894,16 +3437,16 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>-2.7818965817224161E-2</v>
+        <v>-4.4285051651081382E-2</v>
       </c>
       <c r="C9">
-        <v>4.7911550307138482E-3</v>
+        <v>6.5594176085053317E-3</v>
       </c>
       <c r="D9">
-        <v>-5.8063171905083042</v>
+        <v>-6.7513694498820653</v>
       </c>
       <c r="E9">
-        <v>6.3861926857811113E-9</v>
+        <v>1.4645618051645221E-11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -2919,7 +3462,7 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>18879</v>
+        <v>10107</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2935,7 +3478,7 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>-20418.331532415988</v>
+        <v>-10983.47506039397</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -2946,7 +3489,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-3154.5156509866429</v>
+        <v>-1876.5022913065211</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
@@ -2957,7 +3500,7 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>34527.631762858698</v>
+        <v>18213.945538174899</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -2968,7 +3511,7 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.84550570912326717</v>
+        <v>0.82915222359150031</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -2979,7 +3522,7 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.84511390433807698</v>
+        <v>0.82842385666245366</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -2990,7 +3533,7 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>6325.0313019732857</v>
+        <v>3769.0045826130431</v>
       </c>
       <c r="C18" t="s">
         <v>16</v>
@@ -3001,7 +3544,7 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>6387.7977457508459</v>
+        <v>3826.7724508696401</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -3012,7 +3555,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>2.523234027337094E-3</v>
+        <v>1.5921379527638689E-2</v>
       </c>
       <c r="C20" t="s">
         <v>25</v>
@@ -3033,6 +3576,572 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>3.812507432149093</v>
+      </c>
+      <c r="C3">
+        <v>0.38444366450150208</v>
+      </c>
+      <c r="D3">
+        <v>9.9169469656696538</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3.968482453385815</v>
+      </c>
+      <c r="C4">
+        <v>0.71192959795259525</v>
+      </c>
+      <c r="D4">
+        <v>5.5742624899970252</v>
+      </c>
+      <c r="E4">
+        <v>2.4858068714550541E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.65657941839849676</v>
+      </c>
+      <c r="C5">
+        <v>0.33975842549856178</v>
+      </c>
+      <c r="D5">
+        <v>1.932488995482692</v>
+      </c>
+      <c r="E5">
+        <v>5.3299179013275737E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>-11.10755475247745</v>
+      </c>
+      <c r="C6">
+        <v>0.82428070006143528</v>
+      </c>
+      <c r="D6">
+        <v>-13.475451689757611</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>2.6699854485026422</v>
+      </c>
+      <c r="C7">
+        <v>0.22239218905060071</v>
+      </c>
+      <c r="D7">
+        <v>12.00575191017677</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>-2.8012608384226839E-2</v>
+      </c>
+      <c r="C8">
+        <v>4.6073986064738739E-2</v>
+      </c>
+      <c r="D8">
+        <v>-0.60799185781031007</v>
+      </c>
+      <c r="E8">
+        <v>0.54319287410761552</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>-0.105189649998854</v>
+      </c>
+      <c r="C9">
+        <v>2.3564482325759029E-2</v>
+      </c>
+      <c r="D9">
+        <v>-4.4639066772058076</v>
+      </c>
+      <c r="E9">
+        <v>8.0478627897395683E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>-151.3958697344564</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>-88.887562215887669</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>125.0166150371375</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0.4128798733294794</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0.3600382732644859</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>193.77512443177531</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>214.289909963518</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>7.3083455968120153E-4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#NULL!</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>-3.165978029861177</v>
+      </c>
+      <c r="C3">
+        <v>0.15582294587106091</v>
+      </c>
+      <c r="D3">
+        <v>-20.317790888647011</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>-5.5582925600822346</v>
+      </c>
+      <c r="C4">
+        <v>1.060900115384251</v>
+      </c>
+      <c r="D4">
+        <v>-5.2392232590803891</v>
+      </c>
+      <c r="E4">
+        <v>1.6125386159693281E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>-4.7293887508154153</v>
+      </c>
+      <c r="C5">
+        <v>0.205717088896751</v>
+      </c>
+      <c r="D5">
+        <v>-22.989770933367069</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>-2.1663895839812288</v>
+      </c>
+      <c r="C6">
+        <v>0.5352350591577415</v>
+      </c>
+      <c r="D6">
+        <v>-4.0475479827317562</v>
+      </c>
+      <c r="E6">
+        <v>5.175697431569759E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>-3.667777560426837</v>
+      </c>
+      <c r="C7">
+        <v>0.11972094442281001</v>
+      </c>
+      <c r="D7">
+        <v>-30.636056022692301</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>-0.15414176555902981</v>
+      </c>
+      <c r="C8">
+        <v>2.313458087702969E-2</v>
+      </c>
+      <c r="D8">
+        <v>-6.6628293971851056</v>
+      </c>
+      <c r="E8">
+        <v>2.6860513813176109E-11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>-6.2320527466123453E-2</v>
+      </c>
+      <c r="C9">
+        <v>8.7830446896477298E-3</v>
+      </c>
+      <c r="D9">
+        <v>-7.0955493986702001</v>
+      </c>
+      <c r="E9">
+        <v>1.2883027977750321E-12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>9406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>-10069.804818002191</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>-1228.9191613987271</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>17681.77131320694</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>0.87795998198478098</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>0.877165527658745</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>2473.8383227974532</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>2531.0311472974931</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>8.1982540656340072E-3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3295,555 +4404,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>-0.1269627740769981</v>
-      </c>
-      <c r="C2">
-        <v>0.5783775478249773</v>
-      </c>
-      <c r="D2">
-        <v>-0.21951539190006439</v>
-      </c>
-      <c r="E2">
-        <v>0.82624859123976124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>-3.2255623081650948</v>
-      </c>
-      <c r="C3">
-        <v>0.21656144723227419</v>
-      </c>
-      <c r="D3">
-        <v>-14.894443814394631</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>-3.110550593875558</v>
-      </c>
-      <c r="C4">
-        <v>0.35780969961802361</v>
-      </c>
-      <c r="D4">
-        <v>-8.6933098716893298</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>-8.3521333434421035</v>
-      </c>
-      <c r="C5">
-        <v>2.131109103184869</v>
-      </c>
-      <c r="D5">
-        <v>-3.919148640001644</v>
-      </c>
-      <c r="E5">
-        <v>8.8862302088266176E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>-2.2827141547702832</v>
-      </c>
-      <c r="C6">
-        <v>0.19658230835799059</v>
-      </c>
-      <c r="D6">
-        <v>-11.6120019844985</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>-3.3743528676811998</v>
-      </c>
-      <c r="C7">
-        <v>0.1611658260846392</v>
-      </c>
-      <c r="D7">
-        <v>-20.93714870985799</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>-1.493257175468663E-2</v>
-      </c>
-      <c r="C8">
-        <v>3.346676778157435E-3</v>
-      </c>
-      <c r="D8">
-        <v>-4.4619103500362503</v>
-      </c>
-      <c r="E8">
-        <v>8.1232211766035789E-6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>2968</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>-3028.8638748948379</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <v>-535.98964123582937</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>4985.7484673180179</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <v>0.82303937602529631</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
-        <v>0.82072827843586005</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17">
-        <v>1085.979282471659</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
-        <v>1127.94878770167</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
-        <v>7.0955165228789373E-4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>5.0360158157419308</v>
-      </c>
-      <c r="C3">
-        <v>1.0807691329374871</v>
-      </c>
-      <c r="D3">
-        <v>4.6596591836910077</v>
-      </c>
-      <c r="E3">
-        <v>3.1673337346216361E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1.9143119566707841E-10</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>-11.460938824138101</v>
-      </c>
-      <c r="C5">
-        <v>2.724032798041172</v>
-      </c>
-      <c r="D5">
-        <v>-4.2073424491729901</v>
-      </c>
-      <c r="E5">
-        <v>2.5839142924644069E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>0.77958296852499054</v>
-      </c>
-      <c r="C6">
-        <v>4.4074630131912214</v>
-      </c>
-      <c r="D6">
-        <v>0.17687793775960331</v>
-      </c>
-      <c r="E6">
-        <v>0.85960426848705107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>5.6453400399000593</v>
-      </c>
-      <c r="C7">
-        <v>0.99898509047521977</v>
-      </c>
-      <c r="D7">
-        <v>5.6510753701184431</v>
-      </c>
-      <c r="E7">
-        <v>1.5944715325844069E-8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>-0.70317853903774519</v>
-      </c>
-      <c r="C8">
-        <v>0.37260265109687568</v>
-      </c>
-      <c r="D8">
-        <v>-1.88720755734752</v>
-      </c>
-      <c r="E8">
-        <v>5.9132414228509227E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>-2.5133286669159961E-2</v>
-      </c>
-      <c r="C9">
-        <v>3.66527703511021E-2</v>
-      </c>
-      <c r="D9">
-        <v>-0.68571315151364098</v>
-      </c>
-      <c r="E9">
-        <v>0.4928940118028442</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>-23.66290446941348</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>-7.4933095139041193</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>32.339189911018707</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>0.68333094850676823</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <v>0.34524903593594458</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>30.986619027808239</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <v>37.167328805726477</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
-        <v>8.3047561910798266E-5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>